<commit_message>
Update `.gitignore` to include new log and output directories for automation. Modify `workflow_automation.log` to enhance logging details during the Mole tool execution process. Update the binary Excel file for GTS submission to reflect recent changes.
</commit_message>
<xml_diff>
--- a/automation/auto-vpo/output/GTS_Submit_filled_20251219_023105.xlsx
+++ b/automation/auto-vpo/output/GTS_Submit_filled_20251219_023105.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/qibai_chen_intel_com/Documents/Documents/AI_Code/automation/auto-vpo/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_05319118562D03348D7C13C01374F5175759016E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A108495-6DD3-4184-951E-14FE7BE88757}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_05319118562D03348D7C13C01374F5175759016E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{591FF2C5-0078-471C-AC94-983163D7702B}"/>
   <bookViews>
-    <workbookView xWindow="8310" yWindow="5050" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1049,16 +1049,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="128">
@@ -1470,59 +1470,59 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.36328125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="29.1" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+    <row r="2" spans="1:8" ht="30">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1531,7 +1531,7 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1540,16 +1540,16 @@
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1557,94 +1557,94 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="1">
         <v>2571315</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="F3:F8"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="F3:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>